<commit_message>
Modify calculation method for saving percentage
</commit_message>
<xml_diff>
--- a/integration_dat_excl_cost.xlsx
+++ b/integration_dat_excl_cost.xlsx
@@ -327,100 +327,100 @@
     <t>{'27CPU2Mem8GB.sh': 10}</t>
   </si>
   <si>
-    <t>58.38%</t>
-  </si>
-  <si>
-    <t>51.81%</t>
-  </si>
-  <si>
-    <t>5.72%</t>
-  </si>
-  <si>
-    <t>4.89%</t>
-  </si>
-  <si>
-    <t>13.52%</t>
-  </si>
-  <si>
-    <t>52.03%</t>
-  </si>
-  <si>
-    <t>56.24%</t>
-  </si>
-  <si>
-    <t>12.75%</t>
-  </si>
-  <si>
-    <t>71.90%</t>
-  </si>
-  <si>
-    <t>28.36%</t>
-  </si>
-  <si>
-    <t>8.19%</t>
-  </si>
-  <si>
-    <t>82.79%</t>
-  </si>
-  <si>
-    <t>3.96%</t>
-  </si>
-  <si>
-    <t>42.87%</t>
-  </si>
-  <si>
-    <t>39.84%</t>
-  </si>
-  <si>
-    <t>85.54%</t>
-  </si>
-  <si>
-    <t>12.39%</t>
-  </si>
-  <si>
-    <t>7.50%</t>
-  </si>
-  <si>
-    <t>5.01%</t>
-  </si>
-  <si>
-    <t>26.39%</t>
-  </si>
-  <si>
-    <t>53.42%</t>
-  </si>
-  <si>
-    <t>43.23%</t>
-  </si>
-  <si>
-    <t>45.12%</t>
-  </si>
-  <si>
-    <t>41.86%</t>
-  </si>
-  <si>
-    <t>47.63%</t>
-  </si>
-  <si>
-    <t>46.30%</t>
-  </si>
-  <si>
-    <t>69.47%</t>
-  </si>
-  <si>
-    <t>49.18%</t>
-  </si>
-  <si>
-    <t>60.13%</t>
-  </si>
-  <si>
-    <t>50.52%</t>
-  </si>
-  <si>
-    <t>100.00%</t>
-  </si>
-  <si>
-    <t>53.56%</t>
+    <t>41.62%</t>
+  </si>
+  <si>
+    <t>48.19%</t>
+  </si>
+  <si>
+    <t>94.28%</t>
+  </si>
+  <si>
+    <t>95.11%</t>
+  </si>
+  <si>
+    <t>86.48%</t>
+  </si>
+  <si>
+    <t>47.97%</t>
+  </si>
+  <si>
+    <t>43.76%</t>
+  </si>
+  <si>
+    <t>87.25%</t>
+  </si>
+  <si>
+    <t>28.10%</t>
+  </si>
+  <si>
+    <t>71.64%</t>
+  </si>
+  <si>
+    <t>91.81%</t>
+  </si>
+  <si>
+    <t>17.21%</t>
+  </si>
+  <si>
+    <t>96.04%</t>
+  </si>
+  <si>
+    <t>57.13%</t>
+  </si>
+  <si>
+    <t>60.16%</t>
+  </si>
+  <si>
+    <t>14.46%</t>
+  </si>
+  <si>
+    <t>87.61%</t>
+  </si>
+  <si>
+    <t>92.50%</t>
+  </si>
+  <si>
+    <t>94.99%</t>
+  </si>
+  <si>
+    <t>73.61%</t>
+  </si>
+  <si>
+    <t>46.58%</t>
+  </si>
+  <si>
+    <t>56.77%</t>
+  </si>
+  <si>
+    <t>54.88%</t>
+  </si>
+  <si>
+    <t>58.14%</t>
+  </si>
+  <si>
+    <t>52.37%</t>
+  </si>
+  <si>
+    <t>53.70%</t>
+  </si>
+  <si>
+    <t>30.53%</t>
+  </si>
+  <si>
+    <t>50.82%</t>
+  </si>
+  <si>
+    <t>39.87%</t>
+  </si>
+  <si>
+    <t>49.48%</t>
+  </si>
+  <si>
+    <t>0.00%</t>
+  </si>
+  <si>
+    <t>46.44%</t>
   </si>
   <si>
     <t>{'28CPU2Mem16GB.sh': 1, '01noThrottling.sh': 10, '24CPU1Mem4GB.sh': 1}</t>
@@ -531,94 +531,94 @@
     <t>{'24CPU1Mem4GB.sh': 12}</t>
   </si>
   <si>
-    <t>48.13%</t>
-  </si>
-  <si>
-    <t>82.86%</t>
-  </si>
-  <si>
-    <t>99.96%</t>
-  </si>
-  <si>
-    <t>99.98%</t>
-  </si>
-  <si>
-    <t>99.80%</t>
-  </si>
-  <si>
-    <t>99.51%</t>
-  </si>
-  <si>
-    <t>30.23%</t>
-  </si>
-  <si>
-    <t>97.27%</t>
-  </si>
-  <si>
-    <t>17.91%</t>
-  </si>
-  <si>
-    <t>90.32%</t>
-  </si>
-  <si>
-    <t>99.90%</t>
-  </si>
-  <si>
-    <t>41.64%</t>
-  </si>
-  <si>
-    <t>89.92%</t>
-  </si>
-  <si>
-    <t>83.10%</t>
-  </si>
-  <si>
-    <t>97.92%</t>
-  </si>
-  <si>
-    <t>96.87%</t>
-  </si>
-  <si>
-    <t>92.05%</t>
-  </si>
-  <si>
-    <t>33.75%</t>
-  </si>
-  <si>
-    <t>99.84%</t>
-  </si>
-  <si>
-    <t>5.54%</t>
-  </si>
-  <si>
-    <t>63.83%</t>
-  </si>
-  <si>
-    <t>98.87%</t>
-  </si>
-  <si>
-    <t>29.49%</t>
-  </si>
-  <si>
-    <t>3.70%</t>
-  </si>
-  <si>
-    <t>15.00%</t>
-  </si>
-  <si>
-    <t>4.11%</t>
-  </si>
-  <si>
-    <t>94.00%</t>
-  </si>
-  <si>
-    <t>2.33%</t>
-  </si>
-  <si>
-    <t>86.50%</t>
-  </si>
-  <si>
-    <t>99.76%</t>
+    <t>51.87%</t>
+  </si>
+  <si>
+    <t>17.14%</t>
+  </si>
+  <si>
+    <t>0.04%</t>
+  </si>
+  <si>
+    <t>0.02%</t>
+  </si>
+  <si>
+    <t>0.20%</t>
+  </si>
+  <si>
+    <t>0.49%</t>
+  </si>
+  <si>
+    <t>69.77%</t>
+  </si>
+  <si>
+    <t>2.73%</t>
+  </si>
+  <si>
+    <t>82.09%</t>
+  </si>
+  <si>
+    <t>9.68%</t>
+  </si>
+  <si>
+    <t>0.10%</t>
+  </si>
+  <si>
+    <t>58.36%</t>
+  </si>
+  <si>
+    <t>10.08%</t>
+  </si>
+  <si>
+    <t>16.90%</t>
+  </si>
+  <si>
+    <t>2.08%</t>
+  </si>
+  <si>
+    <t>3.13%</t>
+  </si>
+  <si>
+    <t>7.95%</t>
+  </si>
+  <si>
+    <t>66.25%</t>
+  </si>
+  <si>
+    <t>0.16%</t>
+  </si>
+  <si>
+    <t>94.46%</t>
+  </si>
+  <si>
+    <t>36.17%</t>
+  </si>
+  <si>
+    <t>1.13%</t>
+  </si>
+  <si>
+    <t>70.51%</t>
+  </si>
+  <si>
+    <t>96.30%</t>
+  </si>
+  <si>
+    <t>85.00%</t>
+  </si>
+  <si>
+    <t>95.89%</t>
+  </si>
+  <si>
+    <t>6.00%</t>
+  </si>
+  <si>
+    <t>97.67%</t>
+  </si>
+  <si>
+    <t>13.50%</t>
+  </si>
+  <si>
+    <t>0.24%</t>
   </si>
   <si>
     <t>activiti_dot-0.2</t>
@@ -795,58 +795,58 @@
     <t>{'28CPU2Mem16GB.sh': 8}</t>
   </si>
   <si>
-    <t>56.58%</t>
-  </si>
-  <si>
-    <t>4.52%</t>
-  </si>
-  <si>
-    <t>8.92%</t>
-  </si>
-  <si>
-    <t>51.98%</t>
-  </si>
-  <si>
-    <t>12.73%</t>
-  </si>
-  <si>
-    <t>75.74%</t>
-  </si>
-  <si>
-    <t>3.69%</t>
-  </si>
-  <si>
-    <t>42.76%</t>
-  </si>
-  <si>
-    <t>39.81%</t>
-  </si>
-  <si>
-    <t>6.78%</t>
-  </si>
-  <si>
-    <t>4.96%</t>
-  </si>
-  <si>
-    <t>22.11%</t>
-  </si>
-  <si>
-    <t>52.49%</t>
-  </si>
-  <si>
-    <t>44.97%</t>
-  </si>
-  <si>
-    <t>40.65%</t>
-  </si>
-  <si>
-    <t>66.56%</t>
-  </si>
-  <si>
-    <t>60.10%</t>
-  </si>
-  <si>
-    <t>53.55%</t>
+    <t>43.42%</t>
+  </si>
+  <si>
+    <t>95.48%</t>
+  </si>
+  <si>
+    <t>91.08%</t>
+  </si>
+  <si>
+    <t>48.02%</t>
+  </si>
+  <si>
+    <t>87.27%</t>
+  </si>
+  <si>
+    <t>24.26%</t>
+  </si>
+  <si>
+    <t>96.31%</t>
+  </si>
+  <si>
+    <t>57.24%</t>
+  </si>
+  <si>
+    <t>60.19%</t>
+  </si>
+  <si>
+    <t>93.22%</t>
+  </si>
+  <si>
+    <t>95.04%</t>
+  </si>
+  <si>
+    <t>77.89%</t>
+  </si>
+  <si>
+    <t>47.51%</t>
+  </si>
+  <si>
+    <t>55.03%</t>
+  </si>
+  <si>
+    <t>59.35%</t>
+  </si>
+  <si>
+    <t>33.44%</t>
+  </si>
+  <si>
+    <t>39.90%</t>
+  </si>
+  <si>
+    <t>46.45%</t>
   </si>
   <si>
     <t>{'27CPU2Mem8GB.sh': 1, '01noThrottling.sh': 11}</t>
@@ -918,40 +918,40 @@
     <t>1-0.2-fast</t>
   </si>
   <si>
-    <t>48.53%</t>
-  </si>
-  <si>
-    <t>30.24%</t>
-  </si>
-  <si>
-    <t>97.17%</t>
-  </si>
-  <si>
-    <t>90.12%</t>
-  </si>
-  <si>
-    <t>53.88%</t>
-  </si>
-  <si>
-    <t>88.15%</t>
-  </si>
-  <si>
-    <t>82.88%</t>
-  </si>
-  <si>
-    <t>98.02%</t>
-  </si>
-  <si>
-    <t>63.85%</t>
-  </si>
-  <si>
-    <t>99.08%</t>
-  </si>
-  <si>
-    <t>15.06%</t>
-  </si>
-  <si>
-    <t>99.83%</t>
+    <t>51.47%</t>
+  </si>
+  <si>
+    <t>69.76%</t>
+  </si>
+  <si>
+    <t>2.83%</t>
+  </si>
+  <si>
+    <t>9.88%</t>
+  </si>
+  <si>
+    <t>46.12%</t>
+  </si>
+  <si>
+    <t>11.85%</t>
+  </si>
+  <si>
+    <t>17.12%</t>
+  </si>
+  <si>
+    <t>1.98%</t>
+  </si>
+  <si>
+    <t>36.15%</t>
+  </si>
+  <si>
+    <t>0.92%</t>
+  </si>
+  <si>
+    <t>84.94%</t>
+  </si>
+  <si>
+    <t>0.17%</t>
   </si>
   <si>
     <t>activiti_dot-0.4</t>
@@ -1113,16 +1113,16 @@
     <t>{'28CPU2Mem16GB.sh': 10}</t>
   </si>
   <si>
-    <t>8.87%</t>
-  </si>
-  <si>
-    <t>51.94%</t>
-  </si>
-  <si>
-    <t>3.65%</t>
-  </si>
-  <si>
-    <t>44.96%</t>
+    <t>91.13%</t>
+  </si>
+  <si>
+    <t>48.06%</t>
+  </si>
+  <si>
+    <t>96.35%</t>
+  </si>
+  <si>
+    <t>55.04%</t>
   </si>
   <si>
     <t>{'29CPU4Mem8GB.sh': 6, '01noThrottling.sh': 5, '26CPU2Mem4GB.sh': 1}</t>
@@ -1182,34 +1182,34 @@
     <t>1-0.4-fast</t>
   </si>
   <si>
-    <t>48.46%</t>
-  </si>
-  <si>
-    <t>97.29%</t>
-  </si>
-  <si>
-    <t>90.05%</t>
-  </si>
-  <si>
-    <t>57.67%</t>
-  </si>
-  <si>
-    <t>88.90%</t>
-  </si>
-  <si>
-    <t>98.00%</t>
-  </si>
-  <si>
-    <t>91.92%</t>
-  </si>
-  <si>
-    <t>33.74%</t>
-  </si>
-  <si>
-    <t>63.84%</t>
-  </si>
-  <si>
-    <t>15.04%</t>
+    <t>51.54%</t>
+  </si>
+  <si>
+    <t>2.71%</t>
+  </si>
+  <si>
+    <t>9.95%</t>
+  </si>
+  <si>
+    <t>42.33%</t>
+  </si>
+  <si>
+    <t>11.10%</t>
+  </si>
+  <si>
+    <t>2.00%</t>
+  </si>
+  <si>
+    <t>8.08%</t>
+  </si>
+  <si>
+    <t>66.26%</t>
+  </si>
+  <si>
+    <t>36.16%</t>
+  </si>
+  <si>
+    <t>84.96%</t>
   </si>
   <si>
     <t>activiti_dot-0.6</t>
@@ -1362,19 +1362,19 @@
     <t>1-0.6-cheap</t>
   </si>
   <si>
-    <t>56.56%</t>
-  </si>
-  <si>
-    <t>7.66%</t>
-  </si>
-  <si>
-    <t>3.59%</t>
-  </si>
-  <si>
-    <t>4.95%</t>
-  </si>
-  <si>
-    <t>44.93%</t>
+    <t>43.44%</t>
+  </si>
+  <si>
+    <t>92.34%</t>
+  </si>
+  <si>
+    <t>96.41%</t>
+  </si>
+  <si>
+    <t>95.05%</t>
+  </si>
+  <si>
+    <t>55.07%</t>
   </si>
   <si>
     <t>{'26CPU2Mem4GB.sh': 1, '27CPU2Mem8GB.sh': 2, '28CPU2Mem16GB.sh': 1, '29CPU4Mem8GB.sh': 5, '01noThrottling.sh': 3}</t>
@@ -1434,28 +1434,28 @@
     <t>1-0.6-fast</t>
   </si>
   <si>
-    <t>48.54%</t>
-  </si>
-  <si>
-    <t>82.85%</t>
-  </si>
-  <si>
-    <t>97.23%</t>
-  </si>
-  <si>
-    <t>76.67%</t>
-  </si>
-  <si>
-    <t>83.03%</t>
-  </si>
-  <si>
-    <t>97.99%</t>
-  </si>
-  <si>
-    <t>92.06%</t>
-  </si>
-  <si>
-    <t>99.86%</t>
+    <t>51.46%</t>
+  </si>
+  <si>
+    <t>17.15%</t>
+  </si>
+  <si>
+    <t>2.77%</t>
+  </si>
+  <si>
+    <t>23.33%</t>
+  </si>
+  <si>
+    <t>16.97%</t>
+  </si>
+  <si>
+    <t>2.01%</t>
+  </si>
+  <si>
+    <t>7.94%</t>
+  </si>
+  <si>
+    <t>0.14%</t>
   </si>
   <si>
     <t>activiti_dot-0.8</t>
@@ -1617,7 +1617,7 @@
     <t>{'27CPU2Mem8GB.sh': 8}</t>
   </si>
   <si>
-    <t>51.78%</t>
+    <t>48.22%</t>
   </si>
   <si>
     <t>{'26CPU2Mem4GB.sh': 1, '27CPU2Mem8GB.sh': 1, '28CPU2Mem16GB.sh': 2, '29CPU4Mem8GB.sh': 6, '01noThrottling.sh': 2}</t>
@@ -1689,22 +1689,22 @@
     <t>{'22CPU05Mem2GB.sh': 8}</t>
   </si>
   <si>
-    <t>99.68%</t>
-  </si>
-  <si>
-    <t>90.35%</t>
-  </si>
-  <si>
-    <t>48.73%</t>
-  </si>
-  <si>
-    <t>76.24%</t>
-  </si>
-  <si>
-    <t>97.93%</t>
-  </si>
-  <si>
-    <t>99.10%</t>
+    <t>0.32%</t>
+  </si>
+  <si>
+    <t>9.65%</t>
+  </si>
+  <si>
+    <t>51.27%</t>
+  </si>
+  <si>
+    <t>23.76%</t>
+  </si>
+  <si>
+    <t>2.07%</t>
+  </si>
+  <si>
+    <t>0.90%</t>
   </si>
   <si>
     <t>activiti_dot-1</t>
@@ -1848,16 +1848,16 @@
     <t>1-1-cheap</t>
   </si>
   <si>
-    <t>56.41%</t>
-  </si>
-  <si>
-    <t>49.21%</t>
-  </si>
-  <si>
-    <t>4.81%</t>
-  </si>
-  <si>
-    <t>52.36%</t>
+    <t>43.59%</t>
+  </si>
+  <si>
+    <t>50.79%</t>
+  </si>
+  <si>
+    <t>95.19%</t>
+  </si>
+  <si>
+    <t>47.64%</t>
   </si>
   <si>
     <t>{'29CPU4Mem8GB.sh': 2, '01noThrottling.sh': 8, '26CPU2Mem4GB.sh': 2}</t>
@@ -1902,13 +1902,13 @@
     <t>1-1-fast</t>
   </si>
   <si>
-    <t>48.51%</t>
-  </si>
-  <si>
-    <t>97.30%</t>
-  </si>
-  <si>
-    <t>76.92%</t>
+    <t>51.49%</t>
+  </si>
+  <si>
+    <t>2.70%</t>
+  </si>
+  <si>
+    <t>23.08%</t>
   </si>
 </sst>
 </file>

</xml_diff>